<commit_message>
adding new java automation Project
</commit_message>
<xml_diff>
--- a/src/test/resource/VahakHybrid/IMDBautomationWeb/qa/TestData/UserTestData.xlsx
+++ b/src/test/resource/VahakHybrid/IMDBautomationWeb/qa/TestData/UserTestData.xlsx
@@ -1,31 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr/>
+  <bookViews>
+    <workbookView xWindow="360" yWindow="525" windowWidth="19815" windowHeight="7365" activeTab="3"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="validcredential" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="validcredential1" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="validcredential2" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="UserRegistration1" sheetId="4" r:id="rId7"/>
+    <sheet name="validCredential" sheetId="5" r:id="rId1"/>
+    <sheet name="invalidUN" sheetId="6" r:id="rId2"/>
+    <sheet name="invalidPass" sheetId="7" r:id="rId3"/>
+    <sheet name="userReg" sheetId="8" r:id="rId4"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
   <si>
-    <t>UserName</t>
+    <t>uwillgetjob@gmail.com</t>
+  </si>
+  <si>
+    <t>vahaktestAdmin#123</t>
+  </si>
+  <si>
+    <t>Username</t>
   </si>
   <si>
     <t>Password</t>
   </si>
   <si>
-    <t>uwillgetjob@gmail.com</t>
-  </si>
-  <si>
-    <t>vahaktestAdmin#123</t>
+    <t>password</t>
   </si>
   <si>
     <t>uwill@gmail.com</t>
@@ -40,116 +46,76 @@
     <t>email</t>
   </si>
   <si>
-    <t>password</t>
-  </si>
-  <si>
     <t>vahaktest Userone</t>
   </si>
   <si>
-    <t>vahaktest1user@mailinator.com</t>
+    <t>vahaktest1user@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
-      <b/>
-      <sz val="9.0"/>
+      <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="9.0"/>
-      <color rgb="FF000000"/>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
       <name val="Arial"/>
     </font>
-    <font>
-      <sz val="9.0"/>
-      <color rgb="FF000000"/>
-      <name val="-apple-system-font"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+  <cellXfs count="5">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -339,162 +305,164 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="28.0"/>
-    <col customWidth="1" min="2" max="2" width="21.43"/>
-    <col customWidth="1" min="4" max="4" width="29.57"/>
+    <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:2">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="4"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="5"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="4"/>
-    </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="20.14"/>
-    <col customWidth="1" min="2" max="2" width="22.43"/>
+    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
+    <row r="1" spans="1:2">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="25.14"/>
-    <col customWidth="1" min="2" max="2" width="32.0"/>
+    <col min="1" max="1" width="28.85546875" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:2">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>5</v>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="24.57"/>
-    <col customWidth="1" min="2" max="2" width="29.43"/>
-    <col customWidth="1" min="3" max="3" width="20.86"/>
+    <col min="1" max="1" width="20.5703125" customWidth="1"/>
+    <col min="2" max="2" width="31.42578125" customWidth="1"/>
+    <col min="3" max="3" width="28.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="6" t="s">
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="B1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="4" t="s">
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>3</v>
+      <c r="C2" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>